<commit_message>
Added Solution for Tut6
</commit_message>
<xml_diff>
--- a/tut05/output/0401CS01.xlsx
+++ b/tut05/output/0401CS01.xlsx
@@ -550,10 +550,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>7.959183673469388</v>
+        <v>7.96</v>
       </c>
       <c r="C6" t="n">
-        <v>6.818181818181818</v>
+        <v>6.82</v>
       </c>
       <c r="D6" t="n">
         <v>8</v>
@@ -562,13 +562,13 @@
         <v>8</v>
       </c>
       <c r="F6" t="n">
-        <v>7.928571428571429</v>
+        <v>7.93</v>
       </c>
       <c r="G6" t="n">
         <v>7.25</v>
       </c>
       <c r="H6" t="n">
-        <v>8.682926829268293</v>
+        <v>8.68</v>
       </c>
       <c r="I6" t="n">
         <v>8.949999999999999</v>
@@ -612,28 +612,28 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>7.959183673469388</v>
+        <v>7.96</v>
       </c>
       <c r="C8" t="n">
-        <v>7.419354838709677</v>
+        <v>7.42</v>
       </c>
       <c r="D8" t="n">
-        <v>7.602941176470588</v>
+        <v>7.6</v>
       </c>
       <c r="E8" t="n">
-        <v>7.704918032786885</v>
+        <v>7.7</v>
       </c>
       <c r="F8" t="n">
-        <v>7.746666666666667</v>
+        <v>7.75</v>
       </c>
       <c r="G8" t="n">
-        <v>7.671698113207547</v>
+        <v>7.67</v>
       </c>
       <c r="H8" t="n">
-        <v>7.80718954248366</v>
+        <v>7.81</v>
       </c>
       <c r="I8" t="n">
-        <v>7.939306358381502</v>
+        <v>7.94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>